<commit_message>
-finalized ShareImport -MeroShare -MyShare (Custom list)
</commit_message>
<xml_diff>
--- a/public/templates/my-shares-template.xlsx
+++ b/public/templates/my-shares-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\nepse_laravel\storage\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\nepse_laravel\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05E3556-1250-400B-9E11-AF9A474E54D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F3B440-16E5-4678-BB99-0DE8A0B018AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="500">
   <si>
     <t>SGI</t>
   </si>
@@ -1518,7 +1518,10 @@
     <t>Offering name</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1526,7 +1529,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -2026,13 +2029,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2078,7 +2082,91 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2089,6 +2177,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81451A60-F7CE-456F-838E-89CB43E4D382}" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G12" xr:uid="{42F6D730-E325-42C8-99C9-BD4E6BABFD89}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{9DC52A70-1545-437B-8F97-9A8AE7BB1CC9}" name="Symbol" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{2285488C-9B96-408C-856D-31268C7CEE90}" name="Purchase date" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{66A9EAC4-0F5C-4B0A-96C2-8C13C4959DEA}" name="Quantity" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{69A83274-5561-4314-81DD-07164D800F7F}" name="Unit Cost" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{7933E831-1C09-4276-ACEF-06C7C5488DD9}" name="Effective rate" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{E66E4E22-99F0-4BA7-B89E-B3CCCC28D938}" name="Offering type" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{30DBDD84-8FAF-4571-B1A1-ABF0A49C7D55}" name="Remarks" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2391,16 +2495,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2428,228 +2532,244 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5">
         <v>44134</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <v>100</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="6" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5">
         <v>44115</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>200</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>200</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5">
         <v>44090</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="6">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5">
         <v>44134</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="6">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="5">
         <v>44115</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>10</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>100</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>100</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="5">
         <v>44090</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>10</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>500</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>500</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="5">
         <v>44134</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>250</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>251</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="5">
         <v>44115</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>200</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>200</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="5">
         <v>44090</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>100</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>100</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="5">
         <v>44134</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>10</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>100</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>100</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="5">
         <v>44115</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>200</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>200</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="G12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>